<commit_message>
word and excel updated
</commit_message>
<xml_diff>
--- a/Dokumentáció/Tesztek.xlsx
+++ b/Dokumentáció/Tesztek.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27618"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ötödév\ZáróDolgozat Dokumentáció\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity Projects\ZeroGravity\Dokumentáció\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_A52E79BA81BDF474FBC63801D6D09FCB777325AD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D5757C-623B-4A01-B8FA-C6F69BAC4609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>Teszt</t>
   </si>
@@ -42,18 +42,9 @@
     <t>Regisztráció1</t>
   </si>
   <si>
-    <t>Nem megfelelő játékosnév</t>
-  </si>
-  <si>
-    <t>Hiba</t>
-  </si>
-  <si>
     <t>Regisztráció2</t>
   </si>
   <si>
-    <t>A játékosnév már szerepel az adatbázisban</t>
-  </si>
-  <si>
     <t>Bejelentkezés1</t>
   </si>
   <si>
@@ -118,13 +109,28 @@
   </si>
   <si>
     <t>gameover2 menü betöltése</t>
+  </si>
+  <si>
+    <t>Játékosnév: a</t>
+  </si>
+  <si>
+    <t>Hibaüzenet</t>
+  </si>
+  <si>
+    <t>Játékosnév: Teszteset1</t>
+  </si>
+  <si>
+    <t>Hibaüzenet megjelenése (kevesebb mint 4 karakter)</t>
+  </si>
+  <si>
+    <t>Hibaüzenet megjelenése (a játékosnév már szerepel az adatbázisban)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,7 +178,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -185,6 +191,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1782534</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5061856</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2217964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Kép 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{227B4E56-FC93-4B32-6899-C43CF2F912D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14056177" y="163286"/>
+          <a:ext cx="5061858" cy="2245178"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2354034</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>5061856</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2136320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Kép 2" descr="A képen szöveg, képernyőkép, Betűtípus látható&#10;&#10;Automatikusan generált leírás">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23F9038D-348A-B169-6D01-1F643F49219B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14056178" y="2544534"/>
+          <a:ext cx="5061857" cy="2177143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -452,19 +563,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="89.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="76.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,134 +590,135 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="59.25" customHeight="1">
+    <row r="2" spans="1:4" ht="188.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="54.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="57.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="52.5" customHeight="1">
-      <c r="A5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="54.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="71.25" customHeight="1">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="69.75" customHeight="1">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="64.5" customHeight="1">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="56.25" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>